<commit_message>
Harshit | Updated ANM data upload scripts.
</commit_message>
<xml_diff>
--- a/drishti-tools/upload_forms/examples/8 Dhakshakanye PGHundi.xlsx
+++ b/drishti-tools/upload_forms/examples/8 Dhakshakanye PGHundi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="20550" windowHeight="4035"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20550" windowHeight="4035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EC register" sheetId="3" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EC register'!$B$1:$R$724</definedName>
     <definedName name="House_Hold_Information">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6417" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6605" uniqueCount="1094">
   <si>
     <t/>
   </si>
@@ -3308,6 +3308,12 @@
   </si>
   <si>
     <t>22/08/1988</t>
+  </si>
+  <si>
+    <t>29230040111a</t>
+  </si>
+  <si>
+    <t>29230040039a</t>
   </si>
 </sst>
 </file>
@@ -3443,7 +3449,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
@@ -3451,8 +3457,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3505,8 +3512,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="3"/>
@@ -3514,6 +3527,7 @@
     <cellStyle name="Normal_ANC" xfId="6"/>
     <cellStyle name="Normal_Sheet1" xfId="1"/>
     <cellStyle name="Normal_Sheet1_1" xfId="5"/>
+    <cellStyle name="Normal_Sheet4" xfId="7"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3812,8 +3826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R724"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B463" sqref="B463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3895,8 +3909,8 @@
       <c r="A2" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="B2" s="1">
-        <v>29230040111</v>
+      <c r="B2" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>362</v>
@@ -3930,8 +3944,8 @@
       <c r="A3" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="B3" s="1">
-        <v>29230040111</v>
+      <c r="B3" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>362</v>
@@ -3965,8 +3979,8 @@
       <c r="A4" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="B4" s="1">
-        <v>29230040111</v>
+      <c r="B4" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>362</v>
@@ -4000,8 +4014,8 @@
       <c r="A5" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="B5" s="1">
-        <v>29230040111</v>
+      <c r="B5" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>362</v>
@@ -4035,8 +4049,8 @@
       <c r="A6" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B6" s="1">
-        <v>29230040111</v>
+      <c r="B6" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>362</v>
@@ -4073,8 +4087,8 @@
       <c r="A7" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B7" s="1">
-        <v>29230040111</v>
+      <c r="B7" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>362</v>
@@ -4108,8 +4122,8 @@
       <c r="A8" s="1" t="s">
         <v>994</v>
       </c>
-      <c r="B8" s="1">
-        <v>29230040111</v>
+      <c r="B8" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>362</v>
@@ -4137,8 +4151,8 @@
       <c r="A9" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="B9" s="1">
-        <v>29230040111</v>
+      <c r="B9" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>362</v>
@@ -4172,8 +4186,8 @@
       <c r="A10" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="B10" s="1">
-        <v>29230040111</v>
+      <c r="B10" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>362</v>
@@ -4207,8 +4221,8 @@
       <c r="A11" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B11" s="1">
-        <v>29230040111</v>
+      <c r="B11" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>362</v>
@@ -4245,8 +4259,8 @@
       <c r="A12" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B12" s="1">
-        <v>29230040111</v>
+      <c r="B12" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>362</v>
@@ -4280,8 +4294,8 @@
       <c r="A13" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="B13" s="1">
-        <v>29230040111</v>
+      <c r="B13" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>362</v>
@@ -4315,8 +4329,8 @@
       <c r="A14" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B14" s="1">
-        <v>29230040111</v>
+      <c r="B14" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>362</v>
@@ -4350,8 +4364,8 @@
       <c r="A15" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B15" s="1">
-        <v>29230040111</v>
+      <c r="B15" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>362</v>
@@ -4385,8 +4399,8 @@
       <c r="A16" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="B16" s="1">
-        <v>29230040111</v>
+      <c r="B16" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>362</v>
@@ -4423,8 +4437,8 @@
       <c r="A17" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B17" s="1">
-        <v>29230040111</v>
+      <c r="B17" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>362</v>
@@ -4455,8 +4469,8 @@
       <c r="A18" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="B18" s="1">
-        <v>29230040111</v>
+      <c r="B18" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>362</v>
@@ -4490,8 +4504,8 @@
       <c r="A19" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="B19" s="1">
-        <v>29230040111</v>
+      <c r="B19" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>362</v>
@@ -4525,8 +4539,8 @@
       <c r="A20" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="B20" s="1">
-        <v>29230040111</v>
+      <c r="B20" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>362</v>
@@ -4560,8 +4574,8 @@
       <c r="A21" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B21" s="1">
-        <v>29230040111</v>
+      <c r="B21" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>362</v>
@@ -4595,8 +4609,8 @@
       <c r="A22" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B22" s="1">
-        <v>29230040111</v>
+      <c r="B22" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>362</v>
@@ -4630,8 +4644,8 @@
       <c r="A23" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="B23" s="1">
-        <v>29230040111</v>
+      <c r="B23" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>362</v>
@@ -4665,8 +4679,8 @@
       <c r="A24" s="1" t="s">
         <v>993</v>
       </c>
-      <c r="B24" s="1">
-        <v>29230040111</v>
+      <c r="B24" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>362</v>
@@ -4700,8 +4714,8 @@
       <c r="A25" s="1" t="s">
         <v>991</v>
       </c>
-      <c r="B25" s="1">
-        <v>29230040111</v>
+      <c r="B25" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>362</v>
@@ -4735,8 +4749,8 @@
       <c r="A26" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B26" s="1">
-        <v>29230040111</v>
+      <c r="B26" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>362</v>
@@ -4770,8 +4784,8 @@
       <c r="A27" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="B27" s="1">
-        <v>29230040111</v>
+      <c r="B27" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>362</v>
@@ -4805,8 +4819,8 @@
       <c r="A28" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B28" s="1">
-        <v>29230040111</v>
+      <c r="B28" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>362</v>
@@ -4834,8 +4848,8 @@
       <c r="A29" s="1" t="s">
         <v>969</v>
       </c>
-      <c r="B29" s="1">
-        <v>29230040111</v>
+      <c r="B29" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>362</v>
@@ -4869,8 +4883,8 @@
       <c r="A30" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B30" s="1">
-        <v>29230040111</v>
+      <c r="B30" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>362</v>
@@ -4898,8 +4912,8 @@
       <c r="A31" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B31" s="1">
-        <v>29230040111</v>
+      <c r="B31" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>362</v>
@@ -4933,8 +4947,8 @@
       <c r="A32" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B32" s="1">
-        <v>29230040111</v>
+      <c r="B32" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>362</v>
@@ -4968,8 +4982,8 @@
       <c r="A33" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="B33" s="1">
-        <v>29230040111</v>
+      <c r="B33" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>362</v>
@@ -5003,8 +5017,8 @@
       <c r="A34" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B34" s="1">
-        <v>29230040111</v>
+      <c r="B34" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>362</v>
@@ -5038,8 +5052,8 @@
       <c r="A35" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B35" s="1">
-        <v>29230040111</v>
+      <c r="B35" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>362</v>
@@ -5073,8 +5087,8 @@
       <c r="A36" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B36" s="1">
-        <v>29230040111</v>
+      <c r="B36" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>362</v>
@@ -5108,8 +5122,8 @@
       <c r="A37" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="B37" s="1">
-        <v>29230040111</v>
+      <c r="B37" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>362</v>
@@ -5143,8 +5157,8 @@
       <c r="A38" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="B38" s="1">
-        <v>29230040111</v>
+      <c r="B38" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>362</v>
@@ -5172,8 +5186,8 @@
       <c r="A39" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="B39" s="1">
-        <v>29230040111</v>
+      <c r="B39" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>362</v>
@@ -5207,8 +5221,8 @@
       <c r="A40" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="B40" s="1">
-        <v>29230040111</v>
+      <c r="B40" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>362</v>
@@ -5242,8 +5256,8 @@
       <c r="A41" s="1" t="s">
         <v>993</v>
       </c>
-      <c r="B41" s="1">
-        <v>29230040111</v>
+      <c r="B41" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>362</v>
@@ -5277,8 +5291,8 @@
       <c r="A42" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B42" s="1">
-        <v>29230040111</v>
+      <c r="B42" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>362</v>
@@ -5312,8 +5326,8 @@
       <c r="A43" s="1" t="s">
         <v>993</v>
       </c>
-      <c r="B43" s="1">
-        <v>29230040111</v>
+      <c r="B43" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>362</v>
@@ -5347,8 +5361,8 @@
       <c r="A44" s="1" t="s">
         <v>965</v>
       </c>
-      <c r="B44" s="1">
-        <v>29230040111</v>
+      <c r="B44" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>362</v>
@@ -5376,8 +5390,8 @@
       <c r="A45" s="1" t="s">
         <v>969</v>
       </c>
-      <c r="B45" s="1">
-        <v>29230040111</v>
+      <c r="B45" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>362</v>
@@ -5411,8 +5425,8 @@
       <c r="A46" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B46" s="1">
-        <v>29230040111</v>
+      <c r="B46" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>362</v>
@@ -5446,8 +5460,8 @@
       <c r="A47" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B47" s="1">
-        <v>29230040111</v>
+      <c r="B47" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>362</v>
@@ -5478,8 +5492,8 @@
       <c r="A48" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B48" s="1">
-        <v>29230040111</v>
+      <c r="B48" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>362</v>
@@ -5516,8 +5530,8 @@
       <c r="A49" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="B49" s="1">
-        <v>29230040111</v>
+      <c r="B49" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>362</v>
@@ -5551,8 +5565,8 @@
       <c r="A50" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="B50" s="1">
-        <v>29230040111</v>
+      <c r="B50" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>362</v>
@@ -5586,8 +5600,8 @@
       <c r="A51" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B51" s="1">
-        <v>29230040111</v>
+      <c r="B51" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>362</v>
@@ -5621,8 +5635,8 @@
       <c r="A52" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="B52" s="1">
-        <v>29230040111</v>
+      <c r="B52" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>362</v>
@@ -5659,8 +5673,8 @@
       <c r="A53" s="1" t="s">
         <v>993</v>
       </c>
-      <c r="B53" s="1">
-        <v>29230040111</v>
+      <c r="B53" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>362</v>
@@ -5694,8 +5708,8 @@
       <c r="A54" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B54" s="1">
-        <v>29230040111</v>
+      <c r="B54" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>362</v>
@@ -5729,8 +5743,8 @@
       <c r="A55" s="1" t="s">
         <v>1000</v>
       </c>
-      <c r="B55" s="1">
-        <v>29230040111</v>
+      <c r="B55" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>362</v>
@@ -5764,8 +5778,8 @@
       <c r="A56" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B56" s="1">
-        <v>29230040111</v>
+      <c r="B56" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>362</v>
@@ -5793,8 +5807,8 @@
       <c r="A57" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="B57" s="1">
-        <v>29230040111</v>
+      <c r="B57" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>362</v>
@@ -5828,8 +5842,8 @@
       <c r="A58" s="1" t="s">
         <v>994</v>
       </c>
-      <c r="B58" s="1">
-        <v>29230040111</v>
+      <c r="B58" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>362</v>
@@ -5863,8 +5877,8 @@
       <c r="A59" s="1" t="s">
         <v>994</v>
       </c>
-      <c r="B59" s="1">
-        <v>29230040111</v>
+      <c r="B59" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>362</v>
@@ -5898,8 +5912,8 @@
       <c r="A60" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="B60" s="1">
-        <v>29230040111</v>
+      <c r="B60" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>362</v>
@@ -5933,8 +5947,8 @@
       <c r="A61" s="1" t="s">
         <v>960</v>
       </c>
-      <c r="B61" s="1">
-        <v>29230040111</v>
+      <c r="B61" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>362</v>
@@ -5968,8 +5982,8 @@
       <c r="A62" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B62" s="1">
-        <v>29230040111</v>
+      <c r="B62" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>362</v>
@@ -6003,8 +6017,8 @@
       <c r="A63" s="1" t="s">
         <v>1000</v>
       </c>
-      <c r="B63" s="1">
-        <v>29230040111</v>
+      <c r="B63" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>362</v>
@@ -6038,8 +6052,8 @@
       <c r="A64" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B64" s="1">
-        <v>29230040111</v>
+      <c r="B64" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>362</v>
@@ -6073,8 +6087,8 @@
       <c r="A65" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B65" s="1">
-        <v>29230040111</v>
+      <c r="B65" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>362</v>
@@ -6108,8 +6122,8 @@
       <c r="A66" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B66" s="1">
-        <v>29230040111</v>
+      <c r="B66" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>362</v>
@@ -6143,8 +6157,8 @@
       <c r="A67" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B67" s="1">
-        <v>29230040111</v>
+      <c r="B67" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>362</v>
@@ -6178,8 +6192,8 @@
       <c r="A68" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B68" s="1">
-        <v>29230040111</v>
+      <c r="B68" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>362</v>
@@ -6213,8 +6227,8 @@
       <c r="A69" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B69" s="1">
-        <v>29230040111</v>
+      <c r="B69" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>362</v>
@@ -6248,8 +6262,8 @@
       <c r="A70" s="1" t="s">
         <v>967</v>
       </c>
-      <c r="B70" s="1">
-        <v>29230040111</v>
+      <c r="B70" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>362</v>
@@ -6283,8 +6297,8 @@
       <c r="A71" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B71" s="1">
-        <v>29230040111</v>
+      <c r="B71" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>362</v>
@@ -6318,8 +6332,8 @@
       <c r="A72" s="1" t="s">
         <v>969</v>
       </c>
-      <c r="B72" s="1">
-        <v>29230040111</v>
+      <c r="B72" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>362</v>
@@ -6353,8 +6367,8 @@
       <c r="A73" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B73" s="1">
-        <v>29230040111</v>
+      <c r="B73" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>362</v>
@@ -6388,8 +6402,8 @@
       <c r="A74" s="1" t="s">
         <v>991</v>
       </c>
-      <c r="B74" s="1">
-        <v>29230040111</v>
+      <c r="B74" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>362</v>
@@ -6423,8 +6437,8 @@
       <c r="A75" s="1" t="s">
         <v>993</v>
       </c>
-      <c r="B75" s="1">
-        <v>29230040111</v>
+      <c r="B75" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>362</v>
@@ -6461,8 +6475,8 @@
       <c r="A76" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B76" s="1">
-        <v>29230040111</v>
+      <c r="B76" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>362</v>
@@ -6496,8 +6510,8 @@
       <c r="A77" s="1" t="s">
         <v>969</v>
       </c>
-      <c r="B77" s="1">
-        <v>29230040111</v>
+      <c r="B77" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>362</v>
@@ -6534,8 +6548,8 @@
       <c r="A78" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B78" s="1">
-        <v>29230040111</v>
+      <c r="B78" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>362</v>
@@ -6572,8 +6586,8 @@
       <c r="A79" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B79" s="1">
-        <v>29230040111</v>
+      <c r="B79" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>362</v>
@@ -6607,8 +6621,8 @@
       <c r="A80" s="1" t="s">
         <v>965</v>
       </c>
-      <c r="B80" s="1">
-        <v>29230040111</v>
+      <c r="B80" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>362</v>
@@ -6642,8 +6656,8 @@
       <c r="A81" s="1" t="s">
         <v>965</v>
       </c>
-      <c r="B81" s="1">
-        <v>29230040111</v>
+      <c r="B81" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>362</v>
@@ -6677,8 +6691,8 @@
       <c r="A82" s="1" t="s">
         <v>991</v>
       </c>
-      <c r="B82" s="1">
-        <v>29230040111</v>
+      <c r="B82" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>362</v>
@@ -6712,8 +6726,8 @@
       <c r="A83" s="1" t="s">
         <v>991</v>
       </c>
-      <c r="B83" s="1">
-        <v>29230040111</v>
+      <c r="B83" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>362</v>
@@ -6747,8 +6761,8 @@
       <c r="A84" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="B84" s="1">
-        <v>29230040111</v>
+      <c r="B84" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>362</v>
@@ -6785,8 +6799,8 @@
       <c r="A85" s="1" t="s">
         <v>969</v>
       </c>
-      <c r="B85" s="1">
-        <v>29230040111</v>
+      <c r="B85" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>362</v>
@@ -6820,8 +6834,8 @@
       <c r="A86" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B86" s="1">
-        <v>29230040111</v>
+      <c r="B86" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>362</v>
@@ -6855,8 +6869,8 @@
       <c r="A87" s="1" t="s">
         <v>994</v>
       </c>
-      <c r="B87" s="1">
-        <v>29230040111</v>
+      <c r="B87" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>362</v>
@@ -6893,8 +6907,8 @@
       <c r="A88" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B88" s="1">
-        <v>29230040111</v>
+      <c r="B88" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>362</v>
@@ -6928,8 +6942,8 @@
       <c r="A89" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B89" s="1">
-        <v>29230040111</v>
+      <c r="B89" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>362</v>
@@ -6960,8 +6974,8 @@
       <c r="A90" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B90" s="1">
-        <v>29230040111</v>
+      <c r="B90" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>362</v>
@@ -6995,8 +7009,8 @@
       <c r="A91" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="B91" s="1">
-        <v>29230040111</v>
+      <c r="B91" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>362</v>
@@ -7024,8 +7038,8 @@
       <c r="A92" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="B92" s="1">
-        <v>29230040111</v>
+      <c r="B92" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>362</v>
@@ -7059,8 +7073,8 @@
       <c r="A93" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="B93" s="1">
-        <v>29230040111</v>
+      <c r="B93" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>362</v>
@@ -7094,8 +7108,8 @@
       <c r="A94" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="B94" s="1">
-        <v>29230040111</v>
+      <c r="B94" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>362</v>
@@ -7129,8 +7143,8 @@
       <c r="A95" s="1" t="s">
         <v>967</v>
       </c>
-      <c r="B95" s="1">
-        <v>29230040111</v>
+      <c r="B95" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>362</v>
@@ -7164,8 +7178,8 @@
       <c r="A96" s="1" t="s">
         <v>967</v>
       </c>
-      <c r="B96" s="1">
-        <v>29230040111</v>
+      <c r="B96" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>362</v>
@@ -7199,8 +7213,8 @@
       <c r="A97" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B97" s="1">
-        <v>29230040111</v>
+      <c r="B97" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>362</v>
@@ -7234,8 +7248,8 @@
       <c r="A98" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B98" s="1">
-        <v>29230040111</v>
+      <c r="B98" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>362</v>
@@ -7272,8 +7286,8 @@
       <c r="A99" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B99" s="1">
-        <v>29230040111</v>
+      <c r="B99" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>362</v>
@@ -7304,8 +7318,8 @@
       <c r="A100" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B100" s="1">
-        <v>29230040111</v>
+      <c r="B100" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>362</v>
@@ -7339,8 +7353,8 @@
       <c r="A101" s="1" t="s">
         <v>993</v>
       </c>
-      <c r="B101" s="1">
-        <v>29230040111</v>
+      <c r="B101" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>362</v>
@@ -7374,8 +7388,8 @@
       <c r="A102" s="1" t="s">
         <v>993</v>
       </c>
-      <c r="B102" s="1">
-        <v>29230040111</v>
+      <c r="B102" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>362</v>
@@ -7403,8 +7417,8 @@
       <c r="A103" s="1" t="s">
         <v>994</v>
       </c>
-      <c r="B103" s="1">
-        <v>29230040111</v>
+      <c r="B103" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>362</v>
@@ -7438,8 +7452,8 @@
       <c r="A104" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B104" s="1">
-        <v>29230040111</v>
+      <c r="B104" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>362</v>
@@ -7476,8 +7490,8 @@
       <c r="A105" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B105" s="1">
-        <v>29230040111</v>
+      <c r="B105" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>362</v>
@@ -7511,8 +7525,8 @@
       <c r="A106" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B106" s="1">
-        <v>29230040111</v>
+      <c r="B106" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>362</v>
@@ -7540,8 +7554,8 @@
       <c r="A107" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B107" s="1">
-        <v>29230040111</v>
+      <c r="B107" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>362</v>
@@ -7575,8 +7589,8 @@
       <c r="A108" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B108" s="1">
-        <v>29230040111</v>
+      <c r="B108" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>362</v>
@@ -7604,8 +7618,8 @@
       <c r="A109" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="B109" s="1">
-        <v>29230040111</v>
+      <c r="B109" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>362</v>
@@ -7639,8 +7653,8 @@
       <c r="A110" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="B110" s="1">
-        <v>29230040111</v>
+      <c r="B110" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>362</v>
@@ -7677,8 +7691,8 @@
       <c r="A111" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="B111" s="1">
-        <v>29230040111</v>
+      <c r="B111" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>362</v>
@@ -18837,6 +18851,9 @@
       <c r="A435" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B435" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C435" s="1" t="s">
         <v>411</v>
       </c>
@@ -18866,6 +18883,9 @@
       <c r="A436" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B436" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C436" s="1" t="s">
         <v>411</v>
       </c>
@@ -18898,6 +18918,9 @@
       <c r="A437" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B437" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C437" s="1" t="s">
         <v>411</v>
       </c>
@@ -18930,6 +18953,9 @@
       <c r="A438" s="1" t="s">
         <v>963</v>
       </c>
+      <c r="B438" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C438" s="1" t="s">
         <v>411</v>
       </c>
@@ -18962,6 +18988,9 @@
       <c r="A439" s="1" t="s">
         <v>963</v>
       </c>
+      <c r="B439" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C439" s="1" t="s">
         <v>411</v>
       </c>
@@ -18994,6 +19023,9 @@
       <c r="A440" s="1" t="s">
         <v>963</v>
       </c>
+      <c r="B440" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C440" s="1" t="s">
         <v>411</v>
       </c>
@@ -19026,6 +19058,9 @@
       <c r="A441" s="1" t="s">
         <v>963</v>
       </c>
+      <c r="B441" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C441" s="1" t="s">
         <v>411</v>
       </c>
@@ -19058,6 +19093,9 @@
       <c r="A442" s="1" t="s">
         <v>1000</v>
       </c>
+      <c r="B442" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C442" s="1" t="s">
         <v>411</v>
       </c>
@@ -19090,6 +19128,9 @@
       <c r="A443" s="1" t="s">
         <v>962</v>
       </c>
+      <c r="B443" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C443" s="1" t="s">
         <v>411</v>
       </c>
@@ -19122,6 +19163,9 @@
       <c r="A444" s="1" t="s">
         <v>999</v>
       </c>
+      <c r="B444" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C444" s="1" t="s">
         <v>411</v>
       </c>
@@ -19154,6 +19198,9 @@
       <c r="A445" s="1" t="s">
         <v>962</v>
       </c>
+      <c r="B445" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C445" s="1" t="s">
         <v>411</v>
       </c>
@@ -19186,6 +19233,9 @@
       <c r="A446" s="1" t="s">
         <v>998</v>
       </c>
+      <c r="B446" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C446" s="1" t="s">
         <v>411</v>
       </c>
@@ -19221,6 +19271,9 @@
       <c r="A447" s="1" t="s">
         <v>962</v>
       </c>
+      <c r="B447" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C447" s="1" t="s">
         <v>411</v>
       </c>
@@ -19253,6 +19306,9 @@
       <c r="A448" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B448" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C448" s="1" t="s">
         <v>411</v>
       </c>
@@ -19285,6 +19341,9 @@
       <c r="A449" s="1" t="s">
         <v>963</v>
       </c>
+      <c r="B449" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C449" s="1" t="s">
         <v>411</v>
       </c>
@@ -19314,6 +19373,9 @@
       <c r="A450" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B450" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C450" s="1" t="s">
         <v>411</v>
       </c>
@@ -19346,6 +19408,9 @@
       <c r="A451" s="1" t="s">
         <v>993</v>
       </c>
+      <c r="B451" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C451" s="1" t="s">
         <v>411</v>
       </c>
@@ -19378,6 +19443,9 @@
       <c r="A452" s="1" t="s">
         <v>999</v>
       </c>
+      <c r="B452" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C452" s="1" t="s">
         <v>411</v>
       </c>
@@ -19410,6 +19478,9 @@
       <c r="A453" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B453" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C453" s="1" t="s">
         <v>411</v>
       </c>
@@ -19445,6 +19516,9 @@
       <c r="A454" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B454" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C454" s="1" t="s">
         <v>411</v>
       </c>
@@ -19477,6 +19551,9 @@
       <c r="A455" s="1" t="s">
         <v>995</v>
       </c>
+      <c r="B455" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C455" s="1" t="s">
         <v>411</v>
       </c>
@@ -19509,6 +19586,9 @@
       <c r="A456" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B456" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C456" s="1" t="s">
         <v>411</v>
       </c>
@@ -19544,6 +19624,9 @@
       <c r="A457" s="1" t="s">
         <v>994</v>
       </c>
+      <c r="B457" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C457" s="1" t="s">
         <v>411</v>
       </c>
@@ -19573,6 +19656,9 @@
       <c r="A458" s="1" t="s">
         <v>993</v>
       </c>
+      <c r="B458" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C458" s="1" t="s">
         <v>411</v>
       </c>
@@ -19608,6 +19694,9 @@
       <c r="A459" s="1" t="s">
         <v>958</v>
       </c>
+      <c r="B459" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C459" s="1" t="s">
         <v>411</v>
       </c>
@@ -19640,6 +19729,9 @@
       <c r="A460" s="1" t="s">
         <v>958</v>
       </c>
+      <c r="B460" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C460" s="1" t="s">
         <v>411</v>
       </c>
@@ -19672,6 +19764,9 @@
       <c r="A461" s="1" t="s">
         <v>994</v>
       </c>
+      <c r="B461" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C461" s="1" t="s">
         <v>411</v>
       </c>
@@ -19701,6 +19796,9 @@
       <c r="A462" s="1" t="s">
         <v>967</v>
       </c>
+      <c r="B462" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="C462" s="1" t="s">
         <v>411</v>
       </c>
@@ -19727,6 +19825,9 @@
       <c r="A463" s="1" t="s">
         <v>965</v>
       </c>
+      <c r="B463" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C463" s="1" t="s">
         <v>413</v>
       </c>
@@ -19759,6 +19860,9 @@
       <c r="A464" s="1" t="s">
         <v>963</v>
       </c>
+      <c r="B464" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C464" s="1" t="s">
         <v>413</v>
       </c>
@@ -19791,6 +19895,9 @@
       <c r="A465" s="1" t="s">
         <v>960</v>
       </c>
+      <c r="B465" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C465" s="1" t="s">
         <v>413</v>
       </c>
@@ -19823,6 +19930,9 @@
       <c r="A466" s="1" t="s">
         <v>967</v>
       </c>
+      <c r="B466" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C466" s="1" t="s">
         <v>413</v>
       </c>
@@ -19855,6 +19965,9 @@
       <c r="A467" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B467" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C467" s="1" t="s">
         <v>413</v>
       </c>
@@ -19890,6 +20003,9 @@
       <c r="A468" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B468" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C468" s="1" t="s">
         <v>413</v>
       </c>
@@ -19916,6 +20032,9 @@
       <c r="A469" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B469" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C469" s="1" t="s">
         <v>413</v>
       </c>
@@ -19948,6 +20067,9 @@
       <c r="A470" s="1" t="s">
         <v>998</v>
       </c>
+      <c r="B470" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C470" s="1" t="s">
         <v>413</v>
       </c>
@@ -19983,6 +20105,9 @@
       <c r="A471" s="1" t="s">
         <v>998</v>
       </c>
+      <c r="B471" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C471" s="1" t="s">
         <v>413</v>
       </c>
@@ -20009,6 +20134,9 @@
       <c r="A472" s="1" t="s">
         <v>998</v>
       </c>
+      <c r="B472" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C472" s="1" t="s">
         <v>413</v>
       </c>
@@ -20041,6 +20169,9 @@
       <c r="A473" s="1" t="s">
         <v>995</v>
       </c>
+      <c r="B473" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C473" s="1" t="s">
         <v>413</v>
       </c>
@@ -20073,6 +20204,9 @@
       <c r="A474" s="1" t="s">
         <v>995</v>
       </c>
+      <c r="B474" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C474" s="1" t="s">
         <v>413</v>
       </c>
@@ -20105,6 +20239,9 @@
       <c r="A475" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B475" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C475" s="1" t="s">
         <v>413</v>
       </c>
@@ -20137,6 +20274,9 @@
       <c r="A476" s="1" t="s">
         <v>992</v>
       </c>
+      <c r="B476" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C476" s="1" t="s">
         <v>413</v>
       </c>
@@ -20169,6 +20309,9 @@
       <c r="A477" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B477" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C477" s="1" t="s">
         <v>413</v>
       </c>
@@ -20201,6 +20344,9 @@
       <c r="A478" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B478" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C478" s="1" t="s">
         <v>413</v>
       </c>
@@ -20233,6 +20379,9 @@
       <c r="A479" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B479" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C479" s="1" t="s">
         <v>413</v>
       </c>
@@ -20265,6 +20414,9 @@
       <c r="A480" s="1" t="s">
         <v>962</v>
       </c>
+      <c r="B480" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C480" s="1" t="s">
         <v>413</v>
       </c>
@@ -20297,6 +20449,9 @@
       <c r="A481" s="1" t="s">
         <v>995</v>
       </c>
+      <c r="B481" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C481" s="1" t="s">
         <v>413</v>
       </c>
@@ -20329,6 +20484,9 @@
       <c r="A482" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B482" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C482" s="1" t="s">
         <v>413</v>
       </c>
@@ -20361,6 +20519,9 @@
       <c r="A483" s="1" t="s">
         <v>994</v>
       </c>
+      <c r="B483" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C483" s="1" t="s">
         <v>413</v>
       </c>
@@ -20393,6 +20554,9 @@
       <c r="A484" s="1" t="s">
         <v>994</v>
       </c>
+      <c r="B484" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C484" s="1" t="s">
         <v>413</v>
       </c>
@@ -20425,6 +20589,9 @@
       <c r="A485" s="1" t="s">
         <v>967</v>
       </c>
+      <c r="B485" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C485" s="1" t="s">
         <v>413</v>
       </c>
@@ -20457,6 +20624,9 @@
       <c r="A486" s="1" t="s">
         <v>999</v>
       </c>
+      <c r="B486" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C486" s="1" t="s">
         <v>413</v>
       </c>
@@ -20489,6 +20659,9 @@
       <c r="A487" s="1" t="s">
         <v>995</v>
       </c>
+      <c r="B487" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C487" s="1" t="s">
         <v>413</v>
       </c>
@@ -20521,6 +20694,9 @@
       <c r="A488" s="1" t="s">
         <v>992</v>
       </c>
+      <c r="B488" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C488" s="1" t="s">
         <v>413</v>
       </c>
@@ -20553,6 +20729,9 @@
       <c r="A489" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B489" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C489" s="1" t="s">
         <v>413</v>
       </c>
@@ -20585,6 +20764,9 @@
       <c r="A490" s="1" t="s">
         <v>993</v>
       </c>
+      <c r="B490" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C490" s="1" t="s">
         <v>413</v>
       </c>
@@ -20617,6 +20799,9 @@
       <c r="A491" s="1" t="s">
         <v>967</v>
       </c>
+      <c r="B491" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C491" s="1" t="s">
         <v>413</v>
       </c>
@@ -20649,6 +20834,9 @@
       <c r="A492" s="1" t="s">
         <v>969</v>
       </c>
+      <c r="B492" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C492" s="1" t="s">
         <v>413</v>
       </c>
@@ -20675,6 +20863,9 @@
       <c r="A493" s="1" t="s">
         <v>994</v>
       </c>
+      <c r="B493" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C493" s="1" t="s">
         <v>413</v>
       </c>
@@ -20707,6 +20898,9 @@
       <c r="A494" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B494" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C494" s="1" t="s">
         <v>413</v>
       </c>
@@ -20739,6 +20933,9 @@
       <c r="A495" s="1" t="s">
         <v>999</v>
       </c>
+      <c r="B495" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C495" s="1" t="s">
         <v>413</v>
       </c>
@@ -20771,6 +20968,9 @@
       <c r="A496" s="1" t="s">
         <v>963</v>
       </c>
+      <c r="B496" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C496" s="1" t="s">
         <v>413</v>
       </c>
@@ -20803,6 +21003,9 @@
       <c r="A497" s="1" t="s">
         <v>967</v>
       </c>
+      <c r="B497" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C497" s="1" t="s">
         <v>413</v>
       </c>
@@ -20841,6 +21044,9 @@
       <c r="A498" s="1" t="s">
         <v>991</v>
       </c>
+      <c r="B498" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C498" s="1" t="s">
         <v>413</v>
       </c>
@@ -20873,6 +21079,9 @@
       <c r="A499" s="1" t="s">
         <v>963</v>
       </c>
+      <c r="B499" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C499" s="1" t="s">
         <v>413</v>
       </c>
@@ -20905,6 +21114,9 @@
       <c r="A500" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B500" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C500" s="1" t="s">
         <v>413</v>
       </c>
@@ -20937,6 +21149,9 @@
       <c r="A501" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B501" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C501" s="1" t="s">
         <v>413</v>
       </c>
@@ -20969,6 +21184,9 @@
       <c r="A502" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B502" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C502" s="1" t="s">
         <v>413</v>
       </c>
@@ -21001,6 +21219,9 @@
       <c r="A503" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B503" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C503" s="1" t="s">
         <v>413</v>
       </c>
@@ -21036,6 +21257,9 @@
       <c r="A504" s="1" t="s">
         <v>998</v>
       </c>
+      <c r="B504" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C504" s="1" t="s">
         <v>413</v>
       </c>
@@ -21065,6 +21289,9 @@
       <c r="A505" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B505" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C505" s="1" t="s">
         <v>413</v>
       </c>
@@ -21097,6 +21324,9 @@
       <c r="A506" s="1" t="s">
         <v>969</v>
       </c>
+      <c r="B506" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C506" s="1" t="s">
         <v>413</v>
       </c>
@@ -21135,6 +21365,9 @@
       <c r="A507" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B507" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C507" s="1" t="s">
         <v>413</v>
       </c>
@@ -21167,6 +21400,9 @@
       <c r="A508" s="1" t="s">
         <v>962</v>
       </c>
+      <c r="B508" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C508" s="1" t="s">
         <v>413</v>
       </c>
@@ -21199,6 +21435,9 @@
       <c r="A509" s="1" t="s">
         <v>995</v>
       </c>
+      <c r="B509" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C509" s="1" t="s">
         <v>413</v>
       </c>
@@ -21231,6 +21470,9 @@
       <c r="A510" s="1" t="s">
         <v>962</v>
       </c>
+      <c r="B510" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C510" s="1" t="s">
         <v>413</v>
       </c>
@@ -21266,6 +21508,9 @@
       <c r="A511" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B511" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C511" s="1" t="s">
         <v>413</v>
       </c>
@@ -21298,6 +21543,9 @@
       <c r="A512" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B512" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C512" s="1" t="s">
         <v>413</v>
       </c>
@@ -21330,6 +21578,9 @@
       <c r="A513" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B513" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C513" s="1" t="s">
         <v>413</v>
       </c>
@@ -21356,6 +21607,9 @@
       <c r="A514" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B514" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C514" s="1" t="s">
         <v>413</v>
       </c>
@@ -21388,6 +21642,9 @@
       <c r="A515" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B515" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C515" s="1" t="s">
         <v>413</v>
       </c>
@@ -21417,6 +21674,9 @@
       <c r="A516" s="1" t="s">
         <v>999</v>
       </c>
+      <c r="B516" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C516" s="1" t="s">
         <v>413</v>
       </c>
@@ -21449,6 +21709,9 @@
       <c r="A517" s="1" t="s">
         <v>958</v>
       </c>
+      <c r="B517" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C517" s="1" t="s">
         <v>413</v>
       </c>
@@ -21478,6 +21741,9 @@
       <c r="A518" s="1" t="s">
         <v>967</v>
       </c>
+      <c r="B518" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C518" s="1" t="s">
         <v>413</v>
       </c>
@@ -21510,6 +21776,9 @@
       <c r="A519" s="1" t="s">
         <v>992</v>
       </c>
+      <c r="B519" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C519" s="1" t="s">
         <v>413</v>
       </c>
@@ -21542,6 +21811,9 @@
       <c r="A520" s="1" t="s">
         <v>963</v>
       </c>
+      <c r="B520" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C520" s="1" t="s">
         <v>413</v>
       </c>
@@ -21574,6 +21846,9 @@
       <c r="A521" s="1" t="s">
         <v>993</v>
       </c>
+      <c r="B521" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C521" s="1" t="s">
         <v>413</v>
       </c>
@@ -21609,6 +21884,9 @@
       <c r="A522" s="1" t="s">
         <v>998</v>
       </c>
+      <c r="B522" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C522" s="1" t="s">
         <v>413</v>
       </c>
@@ -21644,6 +21922,9 @@
       <c r="A523" s="1" t="s">
         <v>994</v>
       </c>
+      <c r="B523" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C523" s="1" t="s">
         <v>413</v>
       </c>
@@ -21676,6 +21957,9 @@
       <c r="A524" s="1" t="s">
         <v>993</v>
       </c>
+      <c r="B524" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C524" s="1" t="s">
         <v>413</v>
       </c>
@@ -21708,6 +21992,9 @@
       <c r="A525" s="1" t="s">
         <v>967</v>
       </c>
+      <c r="B525" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C525" s="1" t="s">
         <v>413</v>
       </c>
@@ -21740,6 +22027,9 @@
       <c r="A526" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B526" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C526" s="1" t="s">
         <v>413</v>
       </c>
@@ -21772,6 +22062,9 @@
       <c r="A527" s="1" t="s">
         <v>967</v>
       </c>
+      <c r="B527" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C527" s="1" t="s">
         <v>413</v>
       </c>
@@ -21810,6 +22103,9 @@
       <c r="A528" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B528" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C528" s="1" t="s">
         <v>413</v>
       </c>
@@ -21842,6 +22138,9 @@
       <c r="A529" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B529" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C529" s="1" t="s">
         <v>413</v>
       </c>
@@ -21874,6 +22173,9 @@
       <c r="A530" s="1" t="s">
         <v>966</v>
       </c>
+      <c r="B530" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C530" s="1" t="s">
         <v>413</v>
       </c>
@@ -21906,6 +22208,9 @@
       <c r="A531" s="1" t="s">
         <v>993</v>
       </c>
+      <c r="B531" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C531" s="1" t="s">
         <v>413</v>
       </c>
@@ -21938,6 +22243,9 @@
       <c r="A532" s="1" t="s">
         <v>969</v>
       </c>
+      <c r="B532" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C532" s="1" t="s">
         <v>413</v>
       </c>
@@ -21970,6 +22278,9 @@
       <c r="A533" s="1" t="s">
         <v>994</v>
       </c>
+      <c r="B533" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C533" s="1" t="s">
         <v>413</v>
       </c>
@@ -22002,6 +22313,9 @@
       <c r="A534" s="1" t="s">
         <v>994</v>
       </c>
+      <c r="B534" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C534" s="1" t="s">
         <v>413</v>
       </c>
@@ -22028,6 +22342,9 @@
       <c r="A535" s="1" t="s">
         <v>992</v>
       </c>
+      <c r="B535" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C535" s="1" t="s">
         <v>413</v>
       </c>
@@ -22060,6 +22377,9 @@
       <c r="A536" s="1" t="s">
         <v>991</v>
       </c>
+      <c r="B536" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C536" s="1" t="s">
         <v>413</v>
       </c>
@@ -22092,6 +22412,9 @@
       <c r="A537" s="1" t="s">
         <v>958</v>
       </c>
+      <c r="B537" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C537" s="1" t="s">
         <v>413</v>
       </c>
@@ -22124,6 +22447,9 @@
       <c r="A538" s="1" t="s">
         <v>965</v>
       </c>
+      <c r="B538" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="C538" s="1" t="s">
         <v>413</v>
       </c>
@@ -22155,6 +22481,9 @@
     <row r="539" spans="1:15">
       <c r="A539" s="1" t="s">
         <v>963</v>
+      </c>
+      <c r="B539" s="27" t="s">
+        <v>1093</v>
       </c>
       <c r="C539" s="1" t="s">
         <v>413</v>
@@ -28668,9 +28997,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CH17"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15"/>
@@ -29138,8 +29467,8 @@
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9">
-        <v>29230040111</v>
+      <c r="B3" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>362</v>
@@ -29278,8 +29607,8 @@
       <c r="BQ3" s="9" t="s">
         <v>967</v>
       </c>
-      <c r="BR3" s="10">
-        <v>29230040111</v>
+      <c r="BR3" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="BS3" s="9" t="s">
         <v>362</v>
@@ -30673,8 +31002,8 @@
       <c r="A12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>0</v>
+      <c r="B12" s="27">
+        <v>29230040039</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>411</v>
@@ -31025,8 +31354,8 @@
       <c r="A14" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="9">
-        <v>29230040111</v>
+      <c r="B14" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>362</v>
@@ -31165,8 +31494,8 @@
       <c r="BQ14" s="9" t="s">
         <v>967</v>
       </c>
-      <c r="BR14" s="19">
-        <v>29230040111</v>
+      <c r="BR14" s="26" t="s">
+        <v>1092</v>
       </c>
       <c r="BS14" s="13" t="s">
         <v>362</v>
@@ -31217,8 +31546,8 @@
       <c r="A15" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>0</v>
+      <c r="B15" s="27">
+        <v>29230040039</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>411</v>
@@ -31353,7 +31682,9 @@
       <c r="BQ15" s="9" t="s">
         <v>967</v>
       </c>
-      <c r="BR15" s="17"/>
+      <c r="BR15" s="27">
+        <v>29230040039</v>
+      </c>
       <c r="BS15" s="13" t="s">
         <v>411</v>
       </c>
@@ -31597,8 +31928,8 @@
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>0</v>
+      <c r="B17" s="27">
+        <v>29230040039</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>411</v>

</xml_diff>